<commit_message>
working on slime mover
</commit_message>
<xml_diff>
--- a/Assets/Game Notes.xlsx
+++ b/Assets/Game Notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonh\Documents\Unity Projects\Time Slime\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kali VM shared folder\Github Repositories\Slime Time\TimeSlime\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC72B104-2283-4840-A5FC-B5843F5555C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9729AA66-D99F-4680-A182-6D01EC12234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3070" yWindow="2020" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Notes:</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Add slime grappling.  Grappling should be like in DDRace</t>
+  </si>
+  <si>
+    <t>For movement, have every cvircumference point move towards its neighbour</t>
   </si>
 </sst>
 </file>
@@ -351,13 +354,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E1:E3"/>
+  <dimension ref="E1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="73.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
@@ -374,6 +380,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>